<commit_message>
added two cases and update get subscription details
</commit_message>
<xml_diff>
--- a/data/test_cases.xlsx
+++ b/data/test_cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -119,6 +119,15 @@
   </si>
   <si>
     <t>2024-08-27 22:22:10</t>
+  </si>
+  <si>
+    <t>2024-08-28 21:13:20</t>
+  </si>
+  <si>
+    <t>2024-08-28 21:54:08</t>
+  </si>
+  <si>
+    <t>2024-08-28 22:15:06</t>
   </si>
 </sst>
 </file>
@@ -600,9 +609,6 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17">
-        <v>16</v>
-      </c>
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -620,15 +626,45 @@
       <c r="B18" t="s">
         <v>23</v>
       </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18">
+        <v>150</v>
+      </c>
+      <c r="H18" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="B19" t="s">
         <v>24</v>
       </c>
+      <c r="F19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19">
+        <v>75</v>
+      </c>
+      <c r="H19" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
+      <c r="A20">
+        <v>19</v>
+      </c>
       <c r="B20" t="s">
         <v>25</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20">
+        <v>165</v>
+      </c>
+      <c r="H20" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:8">

</xml_diff>